<commit_message>
more buttons and code fixes
</commit_message>
<xml_diff>
--- a/N5NHJ Docs/RGB2RGB565DEC.xlsx
+++ b/N5NHJ Docs/RGB2RGB565DEC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kellercloud-my.sharepoint.com/personal/massimo_mucci_keller-na_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N5NHJ\Documents\GitHub\Nextion8048\N5NHJ Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="546" documentId="11_F25DC773A252ABDACC1048B2B9DF53125ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDEFFE03-6219-40A9-9EBF-1690155EA493}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71274D6-0B4C-44C5-9013-EC248B8F5E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1095" windowWidth="29685" windowHeight="18570" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59745" yWindow="2265" windowWidth="43335" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RGS565" sheetId="1" r:id="rId1"/>
@@ -1167,11 +1167,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1181,7 +1181,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1197,10 +1197,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1469,7 +1465,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,23 +1478,23 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C1">
         <f>_xlfn.BITAND(B1,248)</f>
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D1">
         <f>_xlfn.BITRSHIFT(C1,-8)</f>
-        <v>12288</v>
+        <v>16384</v>
       </c>
       <c r="F1">
         <f>_xlfn.BITAND(D4,63488)</f>
-        <v>12288</v>
+        <v>16384</v>
       </c>
       <c r="G1">
         <f>_xlfn.BITRSHIFT(F1,8)</f>
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1506,23 +1502,23 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <f>_xlfn.BITAND(B2,252)</f>
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <f>_xlfn.BITRSHIFT(C2,-3)</f>
-        <v>416</v>
+        <v>512</v>
       </c>
       <c r="F2">
         <f>_xlfn.BITAND(D4,2016)</f>
-        <v>416</v>
+        <v>512</v>
       </c>
       <c r="G2">
         <f>_xlfn.BITRSHIFT(F2,3)</f>
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,23 +1526,23 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <f>_xlfn.BITAND(B3,B3)</f>
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <f>_xlfn.BITRSHIFT(C3,3)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <f>_xlfn.BITAND(D4,31)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <f>_xlfn.BITRSHIFT(F3,0)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1555,7 +1551,7 @@
       </c>
       <c r="D4">
         <f>SUM(D1:D3)</f>
-        <v>12710</v>
+        <v>16904</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1564,7 +1560,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f>DEC2HEX(D4)</f>
-        <v>31A6</v>
+        <v>4208</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +1853,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
@@ -1914,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AA7129-3EA0-42B1-A672-29B1BB6596F8}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>

</xml_diff>